<commit_message>
change decimal places in summary png
</commit_message>
<xml_diff>
--- a/compare_sml_outcomes.xlsx
+++ b/compare_sml_outcomes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgsri\OneDrive\Desktop\Analysis Projects\Credit_Risk_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47228AD-80F7-44C3-B44B-71BEFF9DF64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECA6173-58AB-42FA-83A9-49A2B520D7EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{F8DE13DD-F2E7-4911-A445-F199E7E09B9F}"/>
   </bookViews>
@@ -141,37 +141,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
@@ -208,6 +190,25 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -222,16 +223,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8B4BAE83-8ECD-4165-BA53-7F6DB976ED77}" name="Table3" displayName="Table3" ref="A3:G18" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8B4BAE83-8ECD-4165-BA53-7F6DB976ED77}" name="Table3" displayName="Table3" ref="A3:G18" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A3:G18" xr:uid="{8B4BAE83-8ECD-4165-BA53-7F6DB976ED77}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{54C1EE8D-0F68-4C76-B9AA-D9D4C4399B55}" name="Column1" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{80A8DFFF-C5C5-4630-9429-8B2883BA617E}" name="Column2" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{9F30EB2A-D399-495C-8203-DBE694BA69A8}" name="Column3" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{3E915E8F-7309-4166-9C10-7A73A44FAE7C}" name="Column4" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{6DE9A487-968E-40B6-A5C9-34E30660C9F7}" name="Column5" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{63682839-E6B6-4F55-A6E1-860330F6C6BD}" name="Column6" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{637044F1-CFED-4F9E-ABA1-1BECCFBB1323}" name="Column7" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{54C1EE8D-0F68-4C76-B9AA-D9D4C4399B55}" name="Column1" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{80A8DFFF-C5C5-4630-9429-8B2883BA617E}" name="Column2" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{9F30EB2A-D399-495C-8203-DBE694BA69A8}" name="Column3" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{3E915E8F-7309-4166-9C10-7A73A44FAE7C}" name="Column4" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{6DE9A487-968E-40B6-A5C9-34E30660C9F7}" name="Column5" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{63682839-E6B6-4F55-A6E1-860330F6C6BD}" name="Column6" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{637044F1-CFED-4F9E-ABA1-1BECCFBB1323}" name="Column7" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -537,7 +538,7 @@
   <dimension ref="A3:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -634,192 +635,192 @@
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="4">
         <v>0.01</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <v>0.01</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="4">
         <v>0.01</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="4">
         <v>0.01</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="4">
         <v>0.03</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="4">
         <v>0.09</v>
       </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="4">
         <v>1</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="4">
         <v>1</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="4">
         <v>1</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="4">
         <v>1</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="4">
         <v>1</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="4">
         <v>1</v>
       </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="4">
         <v>0.71</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="4">
         <v>0.63</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="4">
         <v>0.69</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="4">
         <v>0.65</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="4">
         <v>0.7</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="4">
         <v>0.92</v>
       </c>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="4">
         <v>0.57999999999999996</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="4">
         <v>0.68</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="4">
         <v>0.4</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="4">
         <v>0.6</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="4">
         <v>0.87</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="4">
         <v>0.94</v>
       </c>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="4">
         <v>0.02</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="4">
         <v>0.02</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="4">
         <v>0.01</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="4">
         <v>0.02</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="4">
         <v>0.06</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="4">
         <v>0.16</v>
       </c>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="4">
         <v>0.73</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="4">
         <v>0.81</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="4">
         <v>0.56999999999999995</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="4">
         <v>0.75</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="4">
         <v>0.93</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="4">
         <v>0.97</v>
       </c>
     </row>

</xml_diff>